<commit_message>
auto company postal error
</commit_message>
<xml_diff>
--- a/reference/fix/company_fix/postal_error_fixed.xlsx
+++ b/reference/fix/company_fix/postal_error_fixed.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
@@ -1600,7 +1600,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="19">
     <font>
       <sz val="11"/>
@@ -2688,18 +2688,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2871,7 +2871,7 @@
         <v>16270</v>
       </c>
       <c r="J5" s="1">
-        <v>16430</v>
+        <v>16340</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3895,7 +3895,7 @@
         <v>41326</v>
       </c>
       <c r="J37" s="1">
-        <v>41317</v>
+        <v>41371</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -4055,7 +4055,7 @@
         <v>41326</v>
       </c>
       <c r="J42" s="1">
-        <v>41317</v>
+        <v>41371</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -10711,7 +10711,7 @@
         <v>41326</v>
       </c>
       <c r="J250" s="1">
-        <v>41317</v>
+        <v>41371</v>
       </c>
     </row>
     <row r="251" spans="1:10">

</xml_diff>